<commit_message>
lab 03 - fix excell
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" state="visible" r:id="rId4"/>
@@ -1206,7 +1206,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1333,6 +1333,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="7" fillId="5" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="6" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="7" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2712,7 +2715,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F6" zoomScale="100" workbookViewId="0">
       <selection activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2732,13 +2735,13 @@
     <col customWidth="1" min="13" max="13" width="14.421875"/>
     <col customWidth="1" min="15" max="15" width="11.88671875"/>
     <col customWidth="1" min="16" max="17" width="8.88671875"/>
-    <col customWidth="1" min="21" max="21" width="9.109375"/>
-    <col customWidth="1" min="22" max="22" width="4.00390625"/>
-    <col customWidth="1" min="23" max="24" width="4.28125"/>
-    <col customWidth="1" min="25" max="25" width="5.421875"/>
-    <col customWidth="1" min="26" max="26" width="4.140625"/>
-    <col bestFit="1" customWidth="1" min="27" max="27" width="4.109375"/>
-    <col bestFit="1" customWidth="1" min="28" max="28" width="5.109375"/>
+    <col customWidth="1" min="25" max="25" width="9.109375"/>
+    <col customWidth="1" min="26" max="26" width="4.00390625"/>
+    <col customWidth="1" min="27" max="28" width="4.28125"/>
+    <col customWidth="1" min="29" max="29" width="5.421875"/>
+    <col customWidth="1" min="30" max="30" width="4.140625"/>
+    <col bestFit="1" customWidth="1" min="31" max="31" width="4.109375"/>
+    <col bestFit="1" customWidth="1" min="32" max="32" width="5.109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2798,6 +2801,10 @@
       <c r="Z6" s="35"/>
       <c r="AA6" s="35"/>
       <c r="AB6" s="35"/>
+      <c r="AC6" s="35"/>
+      <c r="AD6" s="35"/>
+      <c r="AE6" s="35"/>
+      <c r="AF6" s="35"/>
     </row>
     <row r="7" ht="15.6">
       <c r="B7" s="35"/>
@@ -2826,15 +2833,19 @@
       <c r="S7" s="41"/>
       <c r="T7" s="41"/>
       <c r="U7" s="41"/>
-      <c r="V7" s="42" t="s">
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
       <c r="AA7" s="42"/>
       <c r="AB7" s="42"/>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="42"/>
+      <c r="AE7" s="42"/>
+      <c r="AF7" s="42"/>
     </row>
     <row r="8" ht="27" customHeight="1">
       <c r="B8" s="35"/>
@@ -2878,35 +2889,47 @@
       <c r="T8" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="U8" s="41" t="s">
+      <c r="U8" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="V8" s="42">
+      <c r="V8" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="W8" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="X8" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y8" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z8" s="42">
         <v>0</v>
       </c>
-      <c r="W8" s="42">
+      <c r="AA8" s="42">
         <v>1</v>
       </c>
-      <c r="X8" s="42">
+      <c r="AB8" s="42">
         <v>2</v>
       </c>
-      <c r="Y8" s="42" t="s">
+      <c r="AC8" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="Z8" s="42" t="s">
+      <c r="AD8" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="AA8" s="42" t="s">
+      <c r="AE8" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AB8" s="42" t="s">
+      <c r="AF8" s="42" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" ht="16.5">
       <c r="B9" s="35"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="38"/>
       <c r="F9" s="39" t="s">
         <v>76</v>
@@ -2914,11 +2937,11 @@
       <c r="G9" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51" t="s">
+      <c r="I9" s="51"/>
+      <c r="J9" s="52" t="s">
         <v>77</v>
       </c>
       <c r="K9" s="45" t="s">
@@ -2928,7 +2951,7 @@
       <c r="M9" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="N9" s="52" t="s">
+      <c r="N9" s="53" t="s">
         <v>76</v>
       </c>
       <c r="O9" s="39" t="s">
@@ -2940,504 +2963,556 @@
       <c r="S9" s="41"/>
       <c r="T9" s="41"/>
       <c r="U9" s="41"/>
-      <c r="V9" s="42"/>
-      <c r="W9" s="42"/>
-      <c r="X9" s="42"/>
-      <c r="Y9" s="42"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
       <c r="Z9" s="42"/>
       <c r="AA9" s="42"/>
       <c r="AB9" s="42"/>
+      <c r="AC9" s="42"/>
+      <c r="AD9" s="42"/>
+      <c r="AE9" s="42"/>
+      <c r="AF9" s="42"/>
     </row>
     <row r="10" ht="16.5">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="56" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G10" s="39"/>
-      <c r="H10" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="O10" s="60"/>
-      <c r="P10" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="61"/>
-      <c r="S10" s="61"/>
-      <c r="T10" s="61"/>
-      <c r="U10" s="61"/>
+      <c r="H10" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="61"/>
+      <c r="P10" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
       <c r="V10" s="62"/>
       <c r="W10" s="62"/>
       <c r="X10" s="62"/>
       <c r="Y10" s="62"/>
-      <c r="Z10" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA10" s="62"/>
-      <c r="AB10" s="62"/>
+      <c r="Z10" s="63"/>
+      <c r="AA10" s="63"/>
+      <c r="AB10" s="63"/>
+      <c r="AC10" s="63"/>
+      <c r="AD10" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE10" s="63"/>
+      <c r="AF10" s="63"/>
     </row>
     <row r="11" ht="16.5">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="56" t="s">
         <v>42</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="39"/>
-      <c r="H11" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11" s="57"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="R11" s="61"/>
-      <c r="S11" s="61"/>
-      <c r="T11" s="61"/>
-      <c r="U11" s="61"/>
+      <c r="H11" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="58"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" s="62"/>
+      <c r="S11" s="62"/>
+      <c r="T11" s="62"/>
+      <c r="U11" s="62"/>
       <c r="V11" s="62"/>
       <c r="W11" s="62"/>
       <c r="X11" s="62"/>
       <c r="Y11" s="62"/>
-      <c r="Z11" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA11" s="62"/>
-      <c r="AB11" s="62"/>
+      <c r="Z11" s="63"/>
+      <c r="AA11" s="63"/>
+      <c r="AB11" s="63"/>
+      <c r="AC11" s="63"/>
+      <c r="AD11" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE11" s="63"/>
+      <c r="AF11" s="63"/>
     </row>
     <row r="12" ht="16.5">
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="56" t="s">
         <v>44</v>
       </c>
       <c r="F12" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G12" s="39"/>
-      <c r="H12" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="N12" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="O12" s="60"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="S12" s="61"/>
-      <c r="T12" s="61"/>
-      <c r="U12" s="61"/>
+      <c r="H12" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="58"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="61"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="S12" s="62"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="62"/>
       <c r="V12" s="62"/>
       <c r="W12" s="62"/>
       <c r="X12" s="62"/>
       <c r="Y12" s="62"/>
-      <c r="Z12" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA12" s="62"/>
-      <c r="AB12" s="62"/>
+      <c r="Z12" s="63"/>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="63"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE12" s="63"/>
+      <c r="AF12" s="63"/>
     </row>
     <row r="13" ht="16.5">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="55" t="s">
+      <c r="E13" s="56" t="s">
         <v>46</v>
       </c>
       <c r="F13" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G13" s="39"/>
-      <c r="H13" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="57"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="N13" s="57"/>
-      <c r="O13" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="61"/>
-      <c r="S13" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="T13" s="61"/>
-      <c r="U13" s="61"/>
+      <c r="H13" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="58"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="58"/>
+      <c r="O13" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="T13" s="62"/>
+      <c r="U13" s="62"/>
       <c r="V13" s="62"/>
       <c r="W13" s="62"/>
       <c r="X13" s="62"/>
       <c r="Y13" s="62"/>
-      <c r="Z13" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA13" s="62"/>
-      <c r="AB13" s="62"/>
+      <c r="Z13" s="63"/>
+      <c r="AA13" s="63"/>
+      <c r="AB13" s="63"/>
+      <c r="AC13" s="63"/>
+      <c r="AD13" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE13" s="63"/>
+      <c r="AF13" s="63"/>
     </row>
     <row r="14" ht="16.5">
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="56" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G14" s="39"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="N14" s="57"/>
-      <c r="O14" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="61"/>
-      <c r="S14" s="61"/>
-      <c r="T14" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="U14" s="61"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="58"/>
+      <c r="O14" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="U14" s="62"/>
       <c r="V14" s="62"/>
       <c r="W14" s="62"/>
       <c r="X14" s="62"/>
       <c r="Y14" s="62"/>
-      <c r="Z14" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA14" s="62"/>
-      <c r="AB14" s="62"/>
+      <c r="Z14" s="63"/>
+      <c r="AA14" s="63"/>
+      <c r="AB14" s="63"/>
+      <c r="AC14" s="63"/>
+      <c r="AD14" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE14" s="63"/>
+      <c r="AF14" s="63"/>
     </row>
     <row r="15" ht="16.5">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="56" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G15" s="39"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="K15" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="O15" s="60"/>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="61"/>
-      <c r="S15" s="61"/>
-      <c r="T15" s="61"/>
-      <c r="U15" s="61" t="s">
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="O15" s="61"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62" t="s">
         <v>80</v>
       </c>
       <c r="V15" s="62"/>
       <c r="W15" s="62"/>
       <c r="X15" s="62"/>
       <c r="Y15" s="62"/>
-      <c r="Z15" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA15" s="62"/>
-      <c r="AB15" s="62"/>
+      <c r="Z15" s="63"/>
+      <c r="AA15" s="63"/>
+      <c r="AB15" s="63"/>
+      <c r="AC15" s="63"/>
+      <c r="AD15" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE15" s="63"/>
+      <c r="AF15" s="63"/>
     </row>
     <row r="16" ht="16.5">
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="56" t="s">
         <v>52</v>
       </c>
       <c r="F16" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G16" s="39"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="K16" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="61"/>
-      <c r="R16" s="61"/>
-      <c r="S16" s="61"/>
-      <c r="T16" s="61"/>
-      <c r="U16" s="61"/>
-      <c r="V16" s="62"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="K16" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="62"/>
+      <c r="T16" s="62"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="62" t="s">
+        <v>80</v>
+      </c>
       <c r="W16" s="62"/>
       <c r="X16" s="62"/>
       <c r="Y16" s="62"/>
-      <c r="Z16" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA16" s="62"/>
-      <c r="AB16" s="62"/>
+      <c r="Z16" s="63"/>
+      <c r="AA16" s="63"/>
+      <c r="AB16" s="63"/>
+      <c r="AC16" s="63"/>
+      <c r="AD16" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE16" s="63"/>
+      <c r="AF16" s="63"/>
     </row>
     <row r="17" ht="16.5">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="64" t="s">
+      <c r="D17" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="56" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G17" s="39"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="K17" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="K17" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="62"/>
       <c r="V17" s="62"/>
-      <c r="W17" s="62"/>
+      <c r="W17" s="62" t="s">
+        <v>80</v>
+      </c>
       <c r="X17" s="62"/>
       <c r="Y17" s="62"/>
-      <c r="Z17" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA17" s="62"/>
-      <c r="AB17" s="62"/>
+      <c r="Z17" s="63"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" ht="16.5">
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="56" t="s">
         <v>56</v>
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="56"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="O18" s="60"/>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="61"/>
-      <c r="R18" s="61"/>
-      <c r="S18" s="61"/>
-      <c r="T18" s="61"/>
-      <c r="U18" s="61"/>
-      <c r="V18" s="62" t="s">
-        <v>80</v>
-      </c>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="O18" s="61"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="62"/>
       <c r="W18" s="62"/>
-      <c r="X18" s="62"/>
+      <c r="X18" s="62" t="s">
+        <v>80</v>
+      </c>
       <c r="Y18" s="62"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="62"/>
-      <c r="AB18" s="62" t="s">
+      <c r="Z18" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" ht="16.5">
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="55" t="s">
+      <c r="E19" s="56" t="s">
         <v>58</v>
       </c>
       <c r="F19" s="39"/>
       <c r="G19" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="56"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="61"/>
-      <c r="S19" s="61"/>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="62" t="s">
-        <v>80</v>
-      </c>
+      <c r="H19" s="57"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="62"/>
+      <c r="U19" s="62"/>
+      <c r="V19" s="62"/>
       <c r="W19" s="62"/>
       <c r="X19" s="62"/>
-      <c r="Y19" s="62"/>
-      <c r="Z19" s="62"/>
-      <c r="AA19" s="62"/>
-      <c r="AB19" s="62" t="s">
+      <c r="Y19" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z19" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA19" s="63"/>
+      <c r="AB19" s="63"/>
+      <c r="AC19" s="63"/>
+      <c r="AD19" s="63"/>
+      <c r="AE19" s="63"/>
+      <c r="AF19" s="63" t="s">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="55">
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:AB6"/>
+    <mergeCell ref="E6:AF6"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:O7"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="V7:AB7"/>
+    <mergeCell ref="P7:Y7"/>
+    <mergeCell ref="Z7:AF7"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:G8"/>
@@ -3457,6 +3532,10 @@
     <mergeCell ref="Z8:Z9"/>
     <mergeCell ref="AA8:AA9"/>
     <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="AC8:AC9"/>
+    <mergeCell ref="AD8:AD9"/>
+    <mergeCell ref="AE8:AE9"/>
+    <mergeCell ref="AF8:AF9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="H10:I10"/>
@@ -3524,364 +3603,364 @@
       <c r="G1" s="4"/>
     </row>
     <row r="3">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
     </row>
     <row r="4">
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="69" t="s">
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="71"/>
+      <c r="L4" s="72"/>
     </row>
     <row r="5" ht="15">
-      <c r="B5" s="72"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="75" t="s">
+      <c r="B5" s="73"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="76" t="s">
+      <c r="I5" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="77"/>
-      <c r="K5" s="78" t="s">
+      <c r="J5" s="78"/>
+      <c r="K5" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="L5" s="75" t="s">
+      <c r="L5" s="76" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" ht="15">
-      <c r="B6" s="79">
+      <c r="B6" s="80">
         <v>9</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="82" t="s">
+      <c r="E6" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="82" t="s">
+      <c r="F6" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="82" t="s">
+      <c r="G6" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="83" t="s">
+      <c r="I6" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="81"/>
-      <c r="K6" s="82" t="s">
+      <c r="J6" s="82"/>
+      <c r="K6" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="L6" s="82" t="s">
+      <c r="L6" s="83" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="79">
+      <c r="B7" s="80">
         <v>10</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81" t="s">
+      <c r="C7" s="81"/>
+      <c r="D7" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="82" t="s">
+      <c r="E7" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="79" t="s">
+      <c r="F7" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="79" t="s">
+      <c r="G7" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="69" t="s">
+      <c r="I7" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="71"/>
-      <c r="K7" s="54" t="s">
+      <c r="J7" s="72"/>
+      <c r="K7" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="L7" s="54" t="s">
+      <c r="L7" s="55" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="79">
+      <c r="B8" s="80">
         <v>11</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="81" t="s">
+      <c r="C8" s="81"/>
+      <c r="D8" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="79" t="s">
+      <c r="G8" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="79" t="s">
+      <c r="H8" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="69" t="s">
+      <c r="I8" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="71"/>
-      <c r="K8" s="82" t="s">
+      <c r="J8" s="72"/>
+      <c r="K8" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="82" t="s">
+      <c r="L8" s="83" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="79">
+      <c r="B9" s="80">
         <v>12</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="81" t="s">
+      <c r="C9" s="81"/>
+      <c r="D9" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="82" t="s">
+      <c r="E9" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="79" t="s">
+      <c r="F9" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="79" t="s">
+      <c r="G9" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="79" t="s">
+      <c r="H9" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="69" t="s">
+      <c r="I9" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="71"/>
-      <c r="K9" s="54" t="s">
+      <c r="J9" s="72"/>
+      <c r="K9" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="L9" s="54" t="s">
+      <c r="L9" s="55" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10" ht="15">
-      <c r="B10" s="75">
+      <c r="B10" s="76">
         <v>13</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="77" t="s">
+      <c r="C10" s="85"/>
+      <c r="D10" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="75" t="s">
+      <c r="E10" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="75" t="s">
+      <c r="F10" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="75" t="s">
+      <c r="G10" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="76" t="s">
+      <c r="I10" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="77"/>
-      <c r="K10" s="75" t="s">
+      <c r="J10" s="78"/>
+      <c r="K10" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="75" t="s">
+      <c r="L10" s="76" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" ht="15">
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="85"/>
-      <c r="L11" s="85"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
     </row>
     <row r="12" ht="15">
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="86" t="s">
         <v>100</v>
       </c>
-      <c r="K12" s="86"/>
+      <c r="K12" s="87"/>
     </row>
     <row r="13" ht="15.6">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="88" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="89" t="s">
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="90"/>
-      <c r="H13" s="87" t="s">
+      <c r="G13" s="91"/>
+      <c r="H13" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="91"/>
-      <c r="M13" s="92" t="s">
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="92"/>
+      <c r="M13" s="93" t="s">
         <v>104</v>
       </c>
-      <c r="N13" s="93"/>
+      <c r="N13" s="94"/>
     </row>
     <row r="14" ht="15">
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="95" t="s">
+      <c r="D14" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="96" t="s">
+      <c r="E14" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="97" t="s">
+      <c r="F14" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="H14" s="99" t="s">
+      <c r="H14" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="95" t="s">
+      <c r="I14" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="J14" s="95" t="s">
+      <c r="J14" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="K14" s="100" t="s">
+      <c r="K14" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="L14" s="101" t="s">
+      <c r="L14" s="102" t="s">
         <v>113</v>
       </c>
-      <c r="M14" s="102" t="s">
+      <c r="M14" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="N14" s="67" t="s">
+      <c r="N14" s="68" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="103"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="107"/>
-      <c r="I15" s="104"/>
-      <c r="J15" s="104"/>
-      <c r="K15" s="108"/>
-      <c r="L15" s="109"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="97"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="110"/>
+      <c r="M15" s="95"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16">
       <c r="B16" s="9">
         <v>5</v>
       </c>
-      <c r="C16" s="110">
+      <c r="C16" s="111">
         <v>5</v>
       </c>
-      <c r="D16" s="110">
+      <c r="D16" s="111">
         <v>0</v>
       </c>
-      <c r="E16" s="111">
+      <c r="E16" s="112">
         <v>1</v>
       </c>
-      <c r="F16" s="112">
+      <c r="F16" s="113">
         <v>0</v>
       </c>
-      <c r="G16" s="113" t="s">
+      <c r="G16" s="114" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="114" t="s">
+      <c r="H16" s="115" t="s">
         <v>117</v>
       </c>
       <c r="I16" s="9">
         <f>SUM(J16:K16)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="110">
+      <c r="J16" s="111">
         <v>0</v>
       </c>
-      <c r="K16" s="115">
+      <c r="K16" s="116">
         <v>0</v>
       </c>
-      <c r="L16" s="116">
+      <c r="L16" s="117">
         <v>100</v>
       </c>
-      <c r="M16" s="117" t="s">
+      <c r="M16" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="N16" s="118">
+      <c r="N16" s="119">
         <f>C16</f>
         <v>5</v>
       </c>

</xml_diff>